<commit_message>
First stab at making presentation more efficient.
</commit_message>
<xml_diff>
--- a/output/TheoryDrivBayes/batch 2 centroid = 0.5/TheoryDrivBayesN1000.xlsx
+++ b/output/TheoryDrivBayes/batch 2 centroid = 0.5/TheoryDrivBayesN1000.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lewan\Documents\MATLAB\Modeling\Replication market\output\TheoryDrivFreq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lewan\Documents\MATLAB\Modeling\Replication market\output\TheoryDrivBayes\batch 2 centroid = 0.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -405,9 +405,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -836,134 +838,6 @@
       </c>
       <c r="J13">
         <v>0.97699999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>